<commit_message>
[SoundSensorRemote] Base sketch separated from remote sketch. First working test.
</commit_message>
<xml_diff>
--- a/sketches/SoundSensorRemote/schematic.xlsx
+++ b/sketches/SoundSensorRemote/schematic.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="37410" windowHeight="18420" tabRatio="427" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" tabRatio="427" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,30 @@
     <author>Joaquim Barrera</author>
   </authors>
   <commentList>
+    <comment ref="Q5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Joaquim Barrera:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Analog Output</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F11" authorId="0" shapeId="0">
       <text>
         <r>
@@ -51,6 +75,78 @@
           </rPr>
           <t xml:space="preserve">
 D2 ocupat pel transceiver</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Joaquim Barrera:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Micro NPN VCC enable.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Joaquim Barrera
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DHT22 NPN vcc enable.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Joaquim Barrera:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Temperature Output</t>
         </r>
       </text>
     </comment>
@@ -123,6 +219,174 @@
           </rPr>
           <t xml:space="preserve">
 CS del transceiver</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AS16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Joaquim Barrera:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Solar 5V</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AV16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Joaquim Barrera:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Solar GND</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Joaquim Barrera:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Micro NPN VCC enable.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Joaquim Barrera
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DHT22 NPN vcc enable.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AR18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Joaquim Barrera:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Diode IN4148</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Joaquim Barrera:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Microphone VCC</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Joaquim Barrera:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Temp VCC</t>
         </r>
       </text>
     </comment>
@@ -131,7 +395,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
   <si>
     <t>rst</t>
   </si>
@@ -139,9 +403,6 @@
     <t>gnd</t>
   </si>
   <si>
-    <t>vin</t>
-  </si>
-  <si>
     <t>3v3</t>
   </si>
   <si>
@@ -187,9 +448,6 @@
     <t>vcc</t>
   </si>
   <si>
-    <t>micro sd card</t>
-  </si>
-  <si>
     <t>csT</t>
   </si>
   <si>
@@ -211,20 +469,74 @@
     <t>do</t>
   </si>
   <si>
-    <t>microphone</t>
-  </si>
-  <si>
-    <t>atmel 328</t>
-  </si>
-  <si>
     <t>flash</t>
+  </si>
+  <si>
+    <t>micro sd card (3,3V o 5V)</t>
+  </si>
+  <si>
+    <t>microphone (2,7 - 5V)</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>tvcc</t>
+  </si>
+  <si>
+    <t>mvcc</t>
+  </si>
+  <si>
+    <t>Solar panel</t>
+  </si>
+  <si>
+    <t>S5V</t>
+  </si>
+  <si>
+    <t>SGND</t>
+  </si>
+  <si>
+    <t>USB LiPo Charger</t>
+  </si>
+  <si>
+    <t>B+</t>
+  </si>
+  <si>
+    <t>B-</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>atmega328</t>
+  </si>
+  <si>
+    <t>BC547</t>
+  </si>
+  <si>
+    <t>DHT22 (3 - 5V)</t>
+  </si>
+  <si>
+    <t>https://cdn-shop.adafruit.com/datasheets/DHT22.pdf</t>
+  </si>
+  <si>
+    <t>men</t>
+  </si>
+  <si>
+    <t>ten</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,8 +571,29 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,7 +656,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -333,8 +690,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -450,11 +825,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -481,31 +870,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -514,7 +879,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -547,6 +912,18 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -610,8 +987,162 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -665,6 +1196,50 @@
         <a:xfrm>
           <a:off x="190502" y="182217"/>
           <a:ext cx="12978560" cy="7523508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="8001000"/>
+          <a:ext cx="9163050" cy="6286500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -941,8 +1516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="AL26:BR49"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BL45" sqref="BL45"/>
+    <sheetView topLeftCell="A10" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1673,10 +2248,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E5:AT15"/>
+  <dimension ref="E5:AY30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1684,74 +2259,81 @@
     <col min="1" max="16384" width="2.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="5" spans="5:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="5:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E5" s="7" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="F5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="21" t="s">
+      <c r="H5" s="13" t="s">
         <v>5</v>
       </c>
+      <c r="I5" s="13" t="s">
+        <v>4</v>
+      </c>
       <c r="J5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="M5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="N5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="O5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="P5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q5" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="R5" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="S5" s="24"/>
-      <c r="T5" s="24"/>
-      <c r="U5" s="24"/>
-      <c r="V5" s="25"/>
-      <c r="AG5" s="19" t="s">
+      <c r="Q5" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="AH5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="AI5" s="11"/>
-      <c r="AJ5" s="11"/>
-      <c r="AK5" s="11"/>
-      <c r="AL5" s="11"/>
-      <c r="AM5" s="12"/>
+      <c r="R5" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="17"/>
+      <c r="AG5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH5" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI5" s="50"/>
+      <c r="AJ5" s="50"/>
+      <c r="AK5" s="50"/>
+      <c r="AL5" s="50"/>
+      <c r="AM5" s="51"/>
       <c r="AN5" s="9"/>
       <c r="AO5" s="9"/>
       <c r="AP5" s="9"/>
-      <c r="AQ5" s="9"/>
-      <c r="AR5" s="9"/>
-      <c r="AS5" s="9"/>
-      <c r="AT5" s="9"/>
-    </row>
-    <row r="6" spans="5:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="22"/>
+      <c r="AQ5" s="77" t="s">
+        <v>30</v>
+      </c>
+      <c r="AR5" s="78"/>
+      <c r="AS5" s="78"/>
+      <c r="AT5" s="78"/>
+      <c r="AU5" s="78"/>
+      <c r="AV5" s="78"/>
+      <c r="AW5" s="78"/>
+      <c r="AX5" s="78"/>
+      <c r="AY5" s="79"/>
+    </row>
+    <row r="6" spans="5:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="14"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -1764,37 +2346,42 @@
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
-      <c r="R6" s="26"/>
-      <c r="S6" s="27"/>
-      <c r="T6" s="27"/>
-      <c r="U6" s="27"/>
-      <c r="V6" s="28"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="20"/>
       <c r="AG6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="AH6" s="13"/>
-      <c r="AI6" s="14"/>
-      <c r="AJ6" s="14"/>
-      <c r="AK6" s="14"/>
-      <c r="AL6" s="14"/>
-      <c r="AM6" s="15"/>
+        <v>6</v>
+      </c>
+      <c r="AH6" s="52"/>
+      <c r="AI6" s="53"/>
+      <c r="AJ6" s="53"/>
+      <c r="AK6" s="53"/>
+      <c r="AL6" s="53"/>
+      <c r="AM6" s="54"/>
       <c r="AN6" s="9"/>
       <c r="AO6" s="9"/>
       <c r="AP6" s="9"/>
-      <c r="AQ6" s="9"/>
-      <c r="AR6" s="9"/>
-      <c r="AS6" s="9"/>
-      <c r="AT6" s="9"/>
-    </row>
-    <row r="7" spans="5:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="22"/>
+      <c r="AQ6" s="80"/>
+      <c r="AR6" s="81"/>
+      <c r="AS6" s="81"/>
+      <c r="AT6" s="81"/>
+      <c r="AU6" s="81"/>
+      <c r="AV6" s="81"/>
+      <c r="AW6" s="81"/>
+      <c r="AX6" s="81"/>
+      <c r="AY6" s="82"/>
+    </row>
+    <row r="7" spans="5:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="14"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="43" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="44"/>
-      <c r="J7" s="45"/>
+      <c r="H7" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="40"/>
+      <c r="J7" s="41"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
@@ -1802,105 +2389,120 @@
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
-      <c r="R7" s="26"/>
-      <c r="S7" s="27"/>
-      <c r="T7" s="27"/>
-      <c r="U7" s="27"/>
-      <c r="V7" s="28"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="20"/>
       <c r="AG7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH7" s="13"/>
-      <c r="AI7" s="14"/>
-      <c r="AJ7" s="14"/>
-      <c r="AK7" s="14"/>
-      <c r="AL7" s="14"/>
-      <c r="AM7" s="15"/>
+        <v>8</v>
+      </c>
+      <c r="AH7" s="52"/>
+      <c r="AI7" s="53"/>
+      <c r="AJ7" s="53"/>
+      <c r="AK7" s="53"/>
+      <c r="AL7" s="53"/>
+      <c r="AM7" s="54"/>
       <c r="AN7" s="9"/>
       <c r="AO7" s="9"/>
       <c r="AP7" s="9"/>
-      <c r="AQ7" s="9"/>
-      <c r="AR7" s="9"/>
-      <c r="AS7" s="9"/>
-      <c r="AT7" s="9"/>
-    </row>
-    <row r="8" spans="5:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="22"/>
+      <c r="AQ7" s="80"/>
+      <c r="AR7" s="81"/>
+      <c r="AS7" s="81"/>
+      <c r="AT7" s="81"/>
+      <c r="AU7" s="81"/>
+      <c r="AV7" s="81"/>
+      <c r="AW7" s="81"/>
+      <c r="AX7" s="81"/>
+      <c r="AY7" s="82"/>
+    </row>
+    <row r="8" spans="5:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="14"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="48"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="44"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="O8" s="47"/>
+      <c r="N8" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="O8" s="43"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
-      <c r="R8" s="26"/>
-      <c r="S8" s="27"/>
-      <c r="T8" s="27"/>
-      <c r="U8" s="27"/>
-      <c r="V8" s="28"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="19"/>
+      <c r="U8" s="19"/>
+      <c r="V8" s="20"/>
       <c r="AG8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH8" s="13"/>
-      <c r="AI8" s="14"/>
-      <c r="AJ8" s="14"/>
-      <c r="AK8" s="14"/>
-      <c r="AL8" s="14"/>
-      <c r="AM8" s="15"/>
+        <v>7</v>
+      </c>
+      <c r="AH8" s="52"/>
+      <c r="AI8" s="53"/>
+      <c r="AJ8" s="53"/>
+      <c r="AK8" s="53"/>
+      <c r="AL8" s="53"/>
+      <c r="AM8" s="54"/>
       <c r="AN8" s="9"/>
       <c r="AO8" s="9"/>
       <c r="AP8" s="9"/>
-      <c r="AQ8" s="9"/>
-      <c r="AR8" s="9"/>
-      <c r="AS8" s="9"/>
-      <c r="AT8" s="9"/>
-    </row>
-    <row r="9" spans="5:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="22"/>
+      <c r="AQ8" s="80"/>
+      <c r="AR8" s="81"/>
+      <c r="AS8" s="81"/>
+      <c r="AT8" s="81"/>
+      <c r="AU8" s="81"/>
+      <c r="AV8" s="81"/>
+      <c r="AW8" s="81"/>
+      <c r="AX8" s="81"/>
+      <c r="AY8" s="82"/>
+    </row>
+    <row r="9" spans="5:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="14"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="51"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="47"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
-      <c r="N9" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="O9" s="52"/>
+      <c r="N9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="O9" s="48"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
-      <c r="R9" s="26"/>
-      <c r="S9" s="27"/>
-      <c r="T9" s="27"/>
-      <c r="U9" s="27"/>
-      <c r="V9" s="28"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19"/>
+      <c r="V9" s="20"/>
       <c r="AG9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="AH9" s="13"/>
-      <c r="AI9" s="14"/>
-      <c r="AJ9" s="14"/>
-      <c r="AK9" s="14"/>
-      <c r="AL9" s="14"/>
-      <c r="AM9" s="15"/>
+        <v>16</v>
+      </c>
+      <c r="AH9" s="52"/>
+      <c r="AI9" s="53"/>
+      <c r="AJ9" s="53"/>
+      <c r="AK9" s="53"/>
+      <c r="AL9" s="53"/>
+      <c r="AM9" s="54"/>
       <c r="AN9" s="9"/>
       <c r="AO9" s="9"/>
       <c r="AP9" s="9"/>
-      <c r="AQ9" s="9"/>
-      <c r="AR9" s="9"/>
-      <c r="AS9" s="9"/>
-      <c r="AT9" s="9"/>
-    </row>
-    <row r="10" spans="5:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AQ9" s="80"/>
+      <c r="AR9" s="81"/>
+      <c r="AS9" s="81"/>
+      <c r="AT9" s="81"/>
+      <c r="AU9" s="81"/>
+      <c r="AV9" s="81"/>
+      <c r="AW9" s="81"/>
+      <c r="AX9" s="81"/>
+      <c r="AY9" s="82"/>
+    </row>
+    <row r="10" spans="5:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E10" s="7" t="s">
         <v>1</v>
       </c>
@@ -1916,73 +2518,78 @@
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
-      <c r="R10" s="26"/>
-      <c r="S10" s="27"/>
-      <c r="T10" s="27"/>
-      <c r="U10" s="27"/>
-      <c r="V10" s="28"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="20"/>
       <c r="AG10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="AH10" s="16"/>
-      <c r="AI10" s="17"/>
-      <c r="AJ10" s="17"/>
-      <c r="AK10" s="17"/>
-      <c r="AL10" s="17"/>
-      <c r="AM10" s="18"/>
+      <c r="AH10" s="55"/>
+      <c r="AI10" s="56"/>
+      <c r="AJ10" s="56"/>
+      <c r="AK10" s="56"/>
+      <c r="AL10" s="56"/>
+      <c r="AM10" s="57"/>
       <c r="AN10" s="9"/>
       <c r="AO10" s="9"/>
       <c r="AP10" s="9"/>
-      <c r="AQ10" s="9"/>
-      <c r="AR10" s="9"/>
-      <c r="AS10" s="9"/>
-      <c r="AT10" s="9"/>
-    </row>
-    <row r="11" spans="5:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AQ10" s="80"/>
+      <c r="AR10" s="81"/>
+      <c r="AS10" s="81"/>
+      <c r="AT10" s="81"/>
+      <c r="AU10" s="81"/>
+      <c r="AV10" s="81"/>
+      <c r="AW10" s="81"/>
+      <c r="AX10" s="81"/>
+      <c r="AY10" s="82"/>
+    </row>
+    <row r="11" spans="5:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="G11" s="5">
+      <c r="F11" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="5">
-        <v>4</v>
+      <c r="G11" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="I11" s="5">
         <v>5</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="58" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="L11" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="N11" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="O11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="P11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q11" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="R11" s="29"/>
-      <c r="S11" s="30"/>
-      <c r="T11" s="30"/>
-      <c r="U11" s="30"/>
-      <c r="V11" s="31"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="22"/>
+      <c r="U11" s="22"/>
+      <c r="V11" s="23"/>
       <c r="AG11" s="9"/>
       <c r="AH11" s="9"/>
       <c r="AI11" s="9"/>
@@ -1993,66 +2600,293 @@
       <c r="AN11" s="9"/>
       <c r="AO11" s="9"/>
       <c r="AP11" s="9"/>
-      <c r="AQ11" s="9"/>
-      <c r="AR11" s="9"/>
-      <c r="AS11" s="9"/>
-      <c r="AT11" s="9"/>
-    </row>
-    <row r="12" spans="5:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AG12" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="AH12" s="35" t="s">
+      <c r="AQ11" s="80"/>
+      <c r="AR11" s="81"/>
+      <c r="AS11" s="81"/>
+      <c r="AT11" s="81"/>
+      <c r="AU11" s="81"/>
+      <c r="AV11" s="81"/>
+      <c r="AW11" s="81"/>
+      <c r="AX11" s="81"/>
+      <c r="AY11" s="82"/>
+    </row>
+    <row r="12" spans="5:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG12" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH12" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="AI12" s="34"/>
-      <c r="AJ12" s="34"/>
-      <c r="AK12" s="34"/>
-      <c r="AL12" s="34"/>
-      <c r="AM12" s="36"/>
-    </row>
-    <row r="13" spans="5:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AG13" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="AH13" s="37"/>
-      <c r="AI13" s="38"/>
-      <c r="AJ13" s="38"/>
-      <c r="AK13" s="38"/>
-      <c r="AL13" s="38"/>
-      <c r="AM13" s="39"/>
-    </row>
-    <row r="14" spans="5:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AG14" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="AH14" s="37"/>
-      <c r="AI14" s="38"/>
-      <c r="AJ14" s="38"/>
-      <c r="AK14" s="38"/>
-      <c r="AL14" s="38"/>
-      <c r="AM14" s="39"/>
-    </row>
-    <row r="15" spans="5:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AI12" s="30"/>
+      <c r="AJ12" s="30"/>
+      <c r="AK12" s="30"/>
+      <c r="AL12" s="30"/>
+      <c r="AM12" s="32"/>
+      <c r="AQ12" s="80"/>
+      <c r="AR12" s="81"/>
+      <c r="AS12" s="81"/>
+      <c r="AT12" s="81"/>
+      <c r="AU12" s="81"/>
+      <c r="AV12" s="81"/>
+      <c r="AW12" s="81"/>
+      <c r="AX12" s="81"/>
+      <c r="AY12" s="82"/>
+    </row>
+    <row r="13" spans="5:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG13" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH13" s="33"/>
+      <c r="AI13" s="34"/>
+      <c r="AJ13" s="34"/>
+      <c r="AK13" s="34"/>
+      <c r="AL13" s="34"/>
+      <c r="AM13" s="35"/>
+      <c r="AQ13" s="80"/>
+      <c r="AR13" s="81"/>
+      <c r="AS13" s="81"/>
+      <c r="AT13" s="81"/>
+      <c r="AU13" s="81"/>
+      <c r="AV13" s="81"/>
+      <c r="AW13" s="81"/>
+      <c r="AX13" s="81"/>
+      <c r="AY13" s="82"/>
+    </row>
+    <row r="14" spans="5:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG14" s="99" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH14" s="33"/>
+      <c r="AI14" s="34"/>
+      <c r="AJ14" s="34"/>
+      <c r="AK14" s="34"/>
+      <c r="AL14" s="34"/>
+      <c r="AM14" s="35"/>
+      <c r="AQ14" s="80"/>
+      <c r="AR14" s="81"/>
+      <c r="AS14" s="81"/>
+      <c r="AT14" s="81"/>
+      <c r="AU14" s="81"/>
+      <c r="AV14" s="81"/>
+      <c r="AW14" s="81"/>
+      <c r="AX14" s="81"/>
+      <c r="AY14" s="82"/>
+    </row>
+    <row r="15" spans="5:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G15" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="66"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="66"/>
+      <c r="K15" s="66"/>
       <c r="AG15" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="AH15" s="40"/>
-      <c r="AI15" s="41"/>
-      <c r="AJ15" s="41"/>
-      <c r="AK15" s="41"/>
-      <c r="AL15" s="41"/>
-      <c r="AM15" s="42"/>
+      <c r="AH15" s="36"/>
+      <c r="AI15" s="37"/>
+      <c r="AJ15" s="37"/>
+      <c r="AK15" s="37"/>
+      <c r="AL15" s="37"/>
+      <c r="AM15" s="38"/>
+      <c r="AQ15" s="83"/>
+      <c r="AR15" s="84"/>
+      <c r="AS15" s="84"/>
+      <c r="AT15" s="84"/>
+      <c r="AU15" s="84"/>
+      <c r="AV15" s="84"/>
+      <c r="AW15" s="84"/>
+      <c r="AX15" s="84"/>
+      <c r="AY15" s="85"/>
+    </row>
+    <row r="16" spans="5:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AS16" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="AT16" s="65"/>
+      <c r="AV16" s="67" t="s">
+        <v>32</v>
+      </c>
+      <c r="AW16" s="67"/>
+    </row>
+    <row r="17" spans="7:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG17" s="99" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH17" s="63"/>
+      <c r="AI17" s="63"/>
+      <c r="AJ17" s="63"/>
+      <c r="AK17" s="63"/>
+      <c r="AL17" s="63"/>
+      <c r="AM17" s="63"/>
+      <c r="AR17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AT17" s="25"/>
+      <c r="AW17" s="25"/>
+    </row>
+    <row r="18" spans="7:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="97"/>
+      <c r="H18" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J18" s="97"/>
+      <c r="K18" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG18" s="58" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH18" s="63"/>
+      <c r="AI18" s="63"/>
+      <c r="AJ18" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="AK18" s="60"/>
+      <c r="AL18" s="63"/>
+      <c r="AM18" s="63"/>
+      <c r="AR18" s="28"/>
+      <c r="AT18" s="25"/>
+      <c r="AW18" s="25"/>
+    </row>
+    <row r="19" spans="7:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="99" t="s">
+        <v>29</v>
+      </c>
+      <c r="J19" s="99" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG19" s="5"/>
+      <c r="AH19" s="63"/>
+      <c r="AJ19" s="61"/>
+      <c r="AK19" s="62"/>
+      <c r="AL19" s="98" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM19" s="63"/>
+      <c r="AR19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AT19" s="26"/>
+      <c r="AW19" s="26"/>
+    </row>
+    <row r="20" spans="7:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH20" s="63"/>
+      <c r="AI20" s="63"/>
+      <c r="AJ20" s="63"/>
+      <c r="AK20" s="63"/>
+      <c r="AL20" s="63"/>
+      <c r="AM20" s="63"/>
+      <c r="AS20" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="AT20" s="65"/>
+      <c r="AV20" s="67" t="s">
+        <v>32</v>
+      </c>
+      <c r="AW20" s="67"/>
+    </row>
+    <row r="21" spans="7:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AS21" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="AT21" s="69"/>
+      <c r="AU21" s="69"/>
+      <c r="AV21" s="69"/>
+      <c r="AW21" s="70"/>
+    </row>
+    <row r="22" spans="7:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AS22" s="71"/>
+      <c r="AT22" s="72"/>
+      <c r="AU22" s="72"/>
+      <c r="AV22" s="72"/>
+      <c r="AW22" s="73"/>
+    </row>
+    <row r="23" spans="7:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AS23" s="74"/>
+      <c r="AT23" s="75"/>
+      <c r="AU23" s="75"/>
+      <c r="AV23" s="75"/>
+      <c r="AW23" s="76"/>
+    </row>
+    <row r="24" spans="7:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AS24" s="95" t="s">
+        <v>34</v>
+      </c>
+      <c r="AT24" s="96"/>
+      <c r="AV24" s="67" t="s">
+        <v>35</v>
+      </c>
+      <c r="AW24" s="67"/>
+    </row>
+    <row r="25" spans="7:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AT25" s="24"/>
+      <c r="AW25" s="25"/>
+    </row>
+    <row r="26" spans="7:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AT26" s="25"/>
+      <c r="AW26" s="25"/>
+    </row>
+    <row r="27" spans="7:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AT27" s="26"/>
+      <c r="AW27" s="25"/>
+    </row>
+    <row r="28" spans="7:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AS28" s="86" t="s">
+        <v>36</v>
+      </c>
+      <c r="AT28" s="87"/>
+      <c r="AU28" s="87"/>
+      <c r="AV28" s="87"/>
+      <c r="AW28" s="88"/>
+    </row>
+    <row r="29" spans="7:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AS29" s="89"/>
+      <c r="AT29" s="90"/>
+      <c r="AU29" s="90"/>
+      <c r="AV29" s="90"/>
+      <c r="AW29" s="91"/>
+    </row>
+    <row r="30" spans="7:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AS30" s="92"/>
+      <c r="AT30" s="93"/>
+      <c r="AU30" s="93"/>
+      <c r="AV30" s="93"/>
+      <c r="AW30" s="94"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="16">
+    <mergeCell ref="AS21:AW23"/>
+    <mergeCell ref="AS24:AT24"/>
+    <mergeCell ref="AV24:AW24"/>
+    <mergeCell ref="AS28:AW30"/>
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="AJ18:AK19"/>
+    <mergeCell ref="AQ5:AY15"/>
+    <mergeCell ref="AS16:AT16"/>
+    <mergeCell ref="AV16:AW16"/>
+    <mergeCell ref="AS20:AT20"/>
+    <mergeCell ref="AV20:AW20"/>
     <mergeCell ref="R5:V11"/>
     <mergeCell ref="AH5:AM10"/>
     <mergeCell ref="AH12:AM15"/>
     <mergeCell ref="H7:J9"/>
     <mergeCell ref="N8:O8"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="AL19" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>